<commit_message>
Version Congres qui compile, avec les calculs fonctionnels
</commit_message>
<xml_diff>
--- a/DonneesConferences/CO2 conférences.xlsx
+++ b/DonneesConferences/CO2 conférences.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkaspari/Documents/Perso/Divers/Programmation/BilanCO2/DonneesConferences/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08BC1FA8-7543-C742-9B46-CBB522438D6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15F67BB5-9F4C-1F47-9B41-8D85ADCA531B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19600" yWindow="500" windowWidth="19200" windowHeight="16240" activeTab="1" xr2:uid="{3BEFCCA0-4A47-A44A-9737-BA198179BEF7}"/>
+    <workbookView xWindow="-38320" yWindow="5360" windowWidth="19200" windowHeight="16240" xr2:uid="{3BEFCCA0-4A47-A44A-9737-BA198179BEF7}"/>
   </bookViews>
   <sheets>
     <sheet name="Collectif" sheetId="1" r:id="rId1"/>
@@ -323,7 +323,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -333,8 +333,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -657,8 +655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00E0F975-A56E-D441-BC3D-3D4EC260A329}">
   <dimension ref="A1:P45"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31:E31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -821,6 +819,10 @@
         <v>4.6912750103598989E-4</v>
       </c>
       <c r="J10" s="8"/>
+      <c r="K10">
+        <f>F10*E10*G10</f>
+        <v>2</v>
+      </c>
       <c r="P10" t="s">
         <v>11</v>
       </c>
@@ -854,6 +856,10 @@
         <v>0.20407046295065562</v>
       </c>
       <c r="J11" s="8"/>
+      <c r="K11">
+        <f>F11*E11*G11</f>
+        <v>580</v>
+      </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
@@ -884,6 +890,10 @@
         <v>0.33542616324073277</v>
       </c>
       <c r="J12" s="8"/>
+      <c r="K12">
+        <f>F12*E12*G12</f>
+        <v>2860</v>
+      </c>
       <c r="P12" t="s">
         <v>13</v>
       </c>
@@ -917,6 +927,10 @@
         <v>5.1604025113958889E-2</v>
       </c>
       <c r="J13" s="8"/>
+      <c r="K13">
+        <f>F13*E13*G13</f>
+        <v>1320</v>
+      </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
@@ -947,6 +961,10 @@
         <v>0.25919294432238443</v>
       </c>
       <c r="J14" s="8"/>
+      <c r="K14">
+        <f>F14*E14*G14</f>
+        <v>6630</v>
+      </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
@@ -1144,7 +1162,7 @@
         <f>D$4*2</f>
         <v>10</v>
       </c>
-      <c r="F23" s="9">
+      <c r="F23">
         <f>0.55/5</f>
         <v>0.11000000000000001</v>
       </c>
@@ -1204,11 +1222,10 @@
       <c r="E27">
         <v>1</v>
       </c>
-      <c r="F27" s="9">
+      <c r="F27">
         <v>6</v>
       </c>
-      <c r="G27" s="9"/>
-      <c r="H27" s="10">
+      <c r="H27" s="6">
         <f>F27*D27*E27</f>
         <v>600</v>
       </c>
@@ -1238,7 +1255,7 @@
       <c r="F28">
         <v>0.9</v>
       </c>
-      <c r="H28" s="10">
+      <c r="H28" s="6">
         <f t="shared" ref="H28:H31" si="5">F28*D28*E28</f>
         <v>450</v>
       </c>
@@ -1271,7 +1288,7 @@
       <c r="F29">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="H29" s="10">
+      <c r="H29" s="6">
         <f t="shared" si="5"/>
         <v>7.0000000000000009</v>
       </c>
@@ -1301,7 +1318,7 @@
       <c r="F30">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="H30" s="10">
+      <c r="H30" s="6">
         <f t="shared" si="5"/>
         <v>250</v>
       </c>
@@ -1331,8 +1348,7 @@
       <c r="F31">
         <v>0.01</v>
       </c>
-      <c r="G31" s="9"/>
-      <c r="H31" s="10">
+      <c r="H31" s="6">
         <f t="shared" si="5"/>
         <v>25</v>
       </c>
@@ -1612,8 +1628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4A32ACA-C7FB-9D48-A4D3-4B05A7AEEF25}">
   <dimension ref="A1:P43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1657,14 +1673,13 @@
       <c r="A7" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9" t="s">
+      <c r="E7" t="s">
         <v>67</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="F7" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="G7" t="s">
         <v>12</v>
       </c>
       <c r="H7" s="6" t="s">
@@ -1675,14 +1690,13 @@
       <c r="B8" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="9"/>
       <c r="E8" s="2">
         <v>15</v>
       </c>
-      <c r="F8" s="9">
+      <c r="F8">
         <v>0.2</v>
       </c>
-      <c r="G8" s="9">
+      <c r="G8">
         <v>4</v>
       </c>
       <c r="H8" s="6">
@@ -1702,12 +1716,11 @@
       <c r="B9" t="s">
         <v>60</v>
       </c>
-      <c r="D9" s="9"/>
       <c r="E9" s="2"/>
-      <c r="F9" s="9">
+      <c r="F9">
         <v>0.1</v>
       </c>
-      <c r="G9" s="9">
+      <c r="G9">
         <v>4</v>
       </c>
       <c r="H9" s="6">
@@ -1724,14 +1737,13 @@
       <c r="B10" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="9"/>
       <c r="E10" s="2">
         <v>1000</v>
       </c>
-      <c r="F10" s="9">
+      <c r="F10">
         <v>2E-3</v>
       </c>
-      <c r="G10" s="9">
+      <c r="G10">
         <v>2</v>
       </c>
       <c r="H10" s="6">
@@ -1751,14 +1763,13 @@
       <c r="B11" t="s">
         <v>65</v>
       </c>
-      <c r="D11" s="9"/>
       <c r="E11" s="2">
         <v>0</v>
       </c>
-      <c r="F11" s="9">
+      <c r="F11">
         <v>0.25</v>
       </c>
-      <c r="G11" s="9">
+      <c r="G11">
         <v>2</v>
       </c>
       <c r="H11" s="6">
@@ -1775,12 +1786,11 @@
       <c r="B12" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="9"/>
       <c r="E12" s="2"/>
-      <c r="F12" s="9">
+      <c r="F12">
         <v>0.6</v>
       </c>
-      <c r="G12" s="9">
+      <c r="G12">
         <v>2</v>
       </c>
       <c r="H12" s="6">
@@ -1797,14 +1807,13 @@
       <c r="B13" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="9"/>
       <c r="E13" s="2">
         <v>10</v>
       </c>
-      <c r="F13" s="9">
+      <c r="F13">
         <v>0.2</v>
       </c>
-      <c r="G13" s="9">
+      <c r="G13">
         <f>4*D$4</f>
         <v>20</v>
       </c>
@@ -1822,12 +1831,11 @@
       <c r="B14" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="9"/>
       <c r="E14" s="2"/>
-      <c r="F14" s="9">
+      <c r="F14">
         <v>0.1</v>
       </c>
-      <c r="G14" s="9">
+      <c r="G14">
         <f>4*D$4</f>
         <v>20</v>
       </c>
@@ -1845,14 +1853,13 @@
       <c r="B15" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="9"/>
       <c r="E15" s="2">
         <v>50</v>
       </c>
-      <c r="F15" s="9">
+      <c r="F15">
         <v>1.2</v>
       </c>
-      <c r="G15" s="9">
+      <c r="G15">
         <f>1/30</f>
         <v>3.3333333333333333E-2</v>
       </c>
@@ -1873,21 +1880,11 @@
       <c r="A16" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
       <c r="J16" s="8">
         <f>SUM(I8:I15)</f>
         <v>0.33646399545193495</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-    </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>24</v>
@@ -1895,15 +1892,13 @@
       <c r="B18" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9">
+      <c r="E18">
         <f>D$4*2-E19-E20</f>
         <v>4</v>
       </c>
-      <c r="F18" s="9">
+      <c r="F18">
         <v>0.51</v>
       </c>
-      <c r="G18" s="9"/>
       <c r="H18" s="6">
         <f>F18*E18</f>
         <v>2.04</v>
@@ -1917,14 +1912,12 @@
       <c r="B19" t="s">
         <v>66</v>
       </c>
-      <c r="D19" s="9"/>
       <c r="E19" s="2">
         <v>3</v>
       </c>
-      <c r="F19" s="9">
+      <c r="F19">
         <v>1.35</v>
       </c>
-      <c r="G19" s="9"/>
       <c r="H19" s="6">
         <f t="shared" ref="H19:H21" si="2">F19*E19</f>
         <v>4.0500000000000007</v>
@@ -1938,14 +1931,12 @@
       <c r="B20" t="s">
         <v>26</v>
       </c>
-      <c r="D20" s="9"/>
       <c r="E20" s="2">
         <v>3</v>
       </c>
-      <c r="F20" s="9">
+      <c r="F20">
         <v>6.29</v>
       </c>
-      <c r="G20" s="9"/>
       <c r="H20" s="6">
         <f t="shared" si="2"/>
         <v>18.87</v>
@@ -1959,16 +1950,14 @@
       <c r="B21" t="s">
         <v>27</v>
       </c>
-      <c r="D21" s="9"/>
       <c r="E21" s="2">
         <f>D$4*2</f>
         <v>10</v>
       </c>
-      <c r="F21" s="9">
+      <c r="F21">
         <f>0.55/5</f>
         <v>0.11000000000000001</v>
       </c>
-      <c r="G21" s="9"/>
       <c r="H21" s="6">
         <f t="shared" si="2"/>
         <v>1.1000000000000001</v>
@@ -1988,30 +1977,19 @@
       <c r="A22" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
       <c r="J22" s="8">
         <f>SUM(I18:I21)</f>
         <v>0.15117675381857631</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-    </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="D24" s="9"/>
-      <c r="E24" s="9" t="s">
+      <c r="E24" t="s">
         <v>4</v>
       </c>
-      <c r="F24" s="9" t="s">
+      <c r="F24" t="s">
         <v>7</v>
       </c>
-      <c r="G24" s="9" t="s">
+      <c r="G24" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2022,15 +2000,13 @@
       <c r="B25" t="s">
         <v>29</v>
       </c>
-      <c r="D25" s="9"/>
       <c r="E25" s="2">
         <v>1</v>
       </c>
-      <c r="F25" s="9">
+      <c r="F25">
         <v>6</v>
       </c>
-      <c r="G25" s="9"/>
-      <c r="H25" s="10">
+      <c r="H25" s="6">
         <f>F25*E25</f>
         <v>6</v>
       </c>
@@ -2047,15 +2023,13 @@
       <c r="B26" t="s">
         <v>41</v>
       </c>
-      <c r="D26" s="9"/>
       <c r="E26" s="2">
         <v>5</v>
       </c>
-      <c r="F26" s="9">
+      <c r="F26">
         <v>0.9</v>
       </c>
-      <c r="G26" s="9"/>
-      <c r="H26" s="10">
+      <c r="H26" s="6">
         <f t="shared" ref="H26:H29" si="4">F26*E26</f>
         <v>4.5</v>
       </c>
@@ -2075,15 +2049,13 @@
       <c r="B27" t="s">
         <v>42</v>
       </c>
-      <c r="D27" s="9"/>
       <c r="E27" s="2">
         <v>3</v>
       </c>
-      <c r="F27" s="9">
+      <c r="F27">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="G27" s="9"/>
-      <c r="H27" s="10">
+      <c r="H27" s="6">
         <f t="shared" si="4"/>
         <v>2.1000000000000001E-2</v>
       </c>
@@ -2100,15 +2072,13 @@
       <c r="B28" t="s">
         <v>40</v>
       </c>
-      <c r="D28" s="9"/>
       <c r="E28" s="2">
         <v>100</v>
       </c>
-      <c r="F28" s="9">
+      <c r="F28">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="G28" s="9"/>
-      <c r="H28" s="10">
+      <c r="H28" s="6">
         <f t="shared" si="4"/>
         <v>2.5</v>
       </c>
@@ -2125,15 +2095,13 @@
       <c r="B29" t="s">
         <v>30</v>
       </c>
-      <c r="D29" s="9"/>
       <c r="E29" s="2">
         <v>5</v>
       </c>
-      <c r="F29" s="9">
+      <c r="F29">
         <v>0.01</v>
       </c>
-      <c r="G29" s="9"/>
-      <c r="H29" s="10">
+      <c r="H29" s="6">
         <f t="shared" si="4"/>
         <v>0.05</v>
       </c>
@@ -2144,14 +2112,12 @@
       <c r="J29" s="8"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="D30" s="9"/>
-      <c r="E30" s="9" t="s">
+      <c r="E30" t="s">
         <v>35</v>
       </c>
-      <c r="F30" s="9" t="s">
+      <c r="F30" t="s">
         <v>7</v>
       </c>
-      <c r="G30" s="9"/>
       <c r="J30" s="8">
         <f>SUM(I25:I29)</f>
         <v>7.5826222147452452E-2</v>
@@ -2161,14 +2127,12 @@
       <c r="B31" t="s">
         <v>31</v>
       </c>
-      <c r="D31" s="9"/>
       <c r="E31" s="2">
         <v>8</v>
       </c>
-      <c r="F31" s="9">
+      <c r="F31">
         <v>0.1</v>
       </c>
-      <c r="G31" s="9"/>
       <c r="H31" s="6">
         <f>E31*F31*D4</f>
         <v>4</v>
@@ -2183,18 +2147,11 @@
       <c r="A32" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D32" s="9"/>
-      <c r="E32" s="9"/>
-      <c r="F32" s="9"/>
-      <c r="G32" s="9"/>
       <c r="I32" s="8"/>
       <c r="J32" s="8"/>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="D33" s="9"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="9"/>
-      <c r="G33" s="9" t="s">
+      <c r="G33" t="s">
         <v>58</v>
       </c>
     </row>
@@ -2205,15 +2162,14 @@
       <c r="B34" t="s">
         <v>33</v>
       </c>
-      <c r="D34" s="9"/>
-      <c r="E34" s="9">
+      <c r="E34">
         <f>D$4</f>
         <v>5</v>
       </c>
-      <c r="F34" s="9">
+      <c r="F34">
         <v>0.1125</v>
       </c>
-      <c r="G34" s="9">
+      <c r="G34">
         <v>20</v>
       </c>
       <c r="H34" s="6">
@@ -2243,14 +2199,12 @@
       <c r="B35" t="s">
         <v>53</v>
       </c>
-      <c r="D35" s="9"/>
       <c r="E35" s="2">
         <v>0</v>
       </c>
-      <c r="F35" s="9">
+      <c r="F35">
         <v>7</v>
       </c>
-      <c r="G35" s="9"/>
       <c r="H35" s="6">
         <f>F35*E35</f>
         <v>0</v>
@@ -2268,15 +2222,13 @@
       <c r="B36" t="s">
         <v>54</v>
       </c>
-      <c r="D36" s="9"/>
       <c r="E36" s="2">
         <f>D$4</f>
         <v>5</v>
       </c>
-      <c r="F36" s="9">
+      <c r="F36">
         <v>12</v>
       </c>
-      <c r="G36" s="9"/>
       <c r="H36" s="6">
         <f>F36*E36</f>
         <v>60</v>
@@ -2291,14 +2243,12 @@
       <c r="B37" t="s">
         <v>55</v>
       </c>
-      <c r="D37" s="9"/>
       <c r="E37" s="2">
         <v>0</v>
       </c>
-      <c r="F37" s="9">
+      <c r="F37">
         <v>50</v>
       </c>
-      <c r="G37" s="9"/>
       <c r="H37" s="6">
         <f>F37*E37</f>
         <v>0</v>
@@ -2313,15 +2263,13 @@
       <c r="B38" t="s">
         <v>34</v>
       </c>
-      <c r="D38" s="9"/>
       <c r="E38" s="2">
         <f>D$4-E35-E36-E37</f>
         <v>0</v>
       </c>
-      <c r="F38" s="9">
+      <c r="F38">
         <v>8.5</v>
       </c>
-      <c r="G38" s="9"/>
       <c r="H38" s="6">
         <f>F38*E38</f>
         <v>0</v>
@@ -2339,10 +2287,6 @@
       <c r="A39" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="D39" s="9"/>
-      <c r="E39" s="9"/>
-      <c r="F39" s="9"/>
-      <c r="G39" s="9"/>
       <c r="J39" s="8">
         <f>SUM(I34:I38)</f>
         <v>0.4133286151025925</v>

</xml_diff>

<commit_message>
Début de mise en place des NSLocalizedStrings Affinage de la base de données
</commit_message>
<xml_diff>
--- a/DonneesConferences/CO2 conférences.xlsx
+++ b/DonneesConferences/CO2 conférences.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkaspari/Documents/Perso/Divers/Programmation/BilanCO2/DonneesConferences/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15F67BB5-9F4C-1F47-9B41-8D85ADCA531B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40B24B3E-5DAC-C24E-B2DC-D8BDE4E19625}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38320" yWindow="5360" windowWidth="19200" windowHeight="16240" xr2:uid="{3BEFCCA0-4A47-A44A-9737-BA198179BEF7}"/>
+    <workbookView xWindow="-38400" yWindow="500" windowWidth="19400" windowHeight="17920" xr2:uid="{3BEFCCA0-4A47-A44A-9737-BA198179BEF7}"/>
   </bookViews>
   <sheets>
     <sheet name="Collectif" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="72">
   <si>
     <t>Informations générales</t>
   </si>
@@ -250,6 +250,9 @@
   </si>
   <si>
     <t>Mieux 0,9 kg CO2 / € (bilan carbone V4) x 5€</t>
+  </si>
+  <si>
+    <t>Nombre max</t>
   </si>
 </sst>
 </file>
@@ -656,7 +659,7 @@
   <dimension ref="A1:P45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -693,7 +696,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
@@ -701,7 +704,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="2">
-        <v>100</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
@@ -736,7 +739,7 @@
       </c>
       <c r="D8">
         <f t="shared" ref="D8:D16" si="0">C8*D$5</f>
-        <v>40</v>
+        <v>30.400000000000002</v>
       </c>
       <c r="E8">
         <v>15</v>
@@ -749,13 +752,17 @@
       </c>
       <c r="H8" s="6">
         <f>F8*E8*D8*G8</f>
-        <v>480</v>
+        <v>364.8</v>
       </c>
       <c r="I8" s="8">
         <f>H8/H$44</f>
-        <v>3.7530200082879191E-3</v>
+        <v>9.723095162606206E-4</v>
       </c>
       <c r="J8" s="8"/>
+      <c r="K8">
+        <f>E8*F8*G8</f>
+        <v>12</v>
+      </c>
       <c r="P8" t="s">
         <v>5</v>
       </c>
@@ -769,7 +776,7 @@
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>7.6000000000000005</v>
       </c>
       <c r="E9">
         <v>15</v>
@@ -782,24 +789,28 @@
       </c>
       <c r="H9" s="6">
         <f t="shared" ref="H9:H17" si="1">F9*E9*D9*G9</f>
-        <v>60</v>
+        <v>45.6</v>
       </c>
       <c r="I9" s="8">
         <f t="shared" ref="I9:I17" si="2">H9/H$44</f>
-        <v>4.6912750103598989E-4</v>
+        <v>1.2153868953257758E-4</v>
       </c>
       <c r="J9" s="8"/>
+      <c r="K9">
+        <f>E9*F9*G9</f>
+        <v>6</v>
+      </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>10</v>
       </c>
       <c r="C10" s="1">
-        <v>0.3</v>
+        <v>0.15</v>
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>11.4</v>
       </c>
       <c r="E10">
         <v>500</v>
@@ -812,11 +823,11 @@
       </c>
       <c r="H10" s="6">
         <f t="shared" si="1"/>
-        <v>60</v>
+        <v>22.8</v>
       </c>
       <c r="I10" s="8">
         <f t="shared" si="2"/>
-        <v>4.6912750103598989E-4</v>
+        <v>6.0769344766288788E-5</v>
       </c>
       <c r="J10" s="8"/>
       <c r="K10">
@@ -832,11 +843,11 @@
         <v>20</v>
       </c>
       <c r="C11" s="1">
-        <v>0.45</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>5.32</v>
       </c>
       <c r="E11">
         <v>1000</v>
@@ -849,11 +860,11 @@
       </c>
       <c r="H11" s="6">
         <f t="shared" si="1"/>
-        <v>26100</v>
+        <v>3085.6000000000004</v>
       </c>
       <c r="I11" s="8">
         <f t="shared" si="2"/>
-        <v>0.20407046295065562</v>
+        <v>8.224117991704416E-3</v>
       </c>
       <c r="J11" s="8"/>
       <c r="K11">
@@ -866,11 +877,11 @@
         <v>21</v>
       </c>
       <c r="C12" s="1">
-        <v>0.15</v>
+        <v>0.05</v>
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>3.8000000000000003</v>
       </c>
       <c r="E12">
         <v>6500</v>
@@ -883,11 +894,11 @@
       </c>
       <c r="H12" s="6">
         <f t="shared" si="1"/>
-        <v>42900</v>
+        <v>10868</v>
       </c>
       <c r="I12" s="8">
         <f t="shared" si="2"/>
-        <v>0.33542616324073277</v>
+        <v>2.8966721005264321E-2</v>
       </c>
       <c r="J12" s="8"/>
       <c r="K12">
@@ -903,11 +914,11 @@
         <v>22</v>
       </c>
       <c r="C13" s="1">
-        <v>0.05</v>
+        <v>0.06</v>
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>4.5599999999999996</v>
       </c>
       <c r="E13">
         <v>1000</v>
@@ -920,11 +931,11 @@
       </c>
       <c r="H13" s="6">
         <f t="shared" si="1"/>
-        <v>6600</v>
+        <v>6019.2</v>
       </c>
       <c r="I13" s="8">
         <f t="shared" si="2"/>
-        <v>5.1604025113958889E-2</v>
+        <v>1.6043107018300237E-2</v>
       </c>
       <c r="J13" s="8"/>
       <c r="K13">
@@ -937,11 +948,11 @@
         <v>23</v>
       </c>
       <c r="C14" s="1">
-        <v>0.05</v>
+        <v>0.67</v>
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>50.92</v>
       </c>
       <c r="E14">
         <v>6500</v>
@@ -954,11 +965,11 @@
       </c>
       <c r="H14" s="6">
         <f t="shared" si="1"/>
-        <v>33150</v>
+        <v>337599.60000000003</v>
       </c>
       <c r="I14" s="8">
         <f t="shared" si="2"/>
-        <v>0.25919294432238443</v>
+        <v>0.89981168795443811</v>
       </c>
       <c r="J14" s="8"/>
       <c r="K14">
@@ -975,7 +986,7 @@
       </c>
       <c r="D15">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="E15">
         <v>10</v>
@@ -985,15 +996,15 @@
       </c>
       <c r="G15">
         <f>4*D$4</f>
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="H15" s="6">
         <f t="shared" si="1"/>
-        <v>2000</v>
+        <v>1824</v>
       </c>
       <c r="I15" s="8">
         <f t="shared" si="2"/>
-        <v>1.5637583367866331E-2</v>
+        <v>4.8615475813031028E-3</v>
       </c>
       <c r="J15" s="8"/>
     </row>
@@ -1006,7 +1017,7 @@
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>7.6000000000000005</v>
       </c>
       <c r="E16">
         <v>10</v>
@@ -1016,15 +1027,15 @@
       </c>
       <c r="G16">
         <f>4*D$4</f>
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="H16" s="6">
         <f t="shared" si="1"/>
-        <v>200</v>
+        <v>182.4</v>
       </c>
       <c r="I16" s="8">
         <f t="shared" si="2"/>
-        <v>1.563758336786633E-3</v>
+        <v>4.861547581303103E-4</v>
       </c>
       <c r="J16" s="8"/>
     </row>
@@ -1060,7 +1071,12 @@
       </c>
       <c r="J18" s="8">
         <f>SUM(I8:I17)</f>
-        <v>0.87218621234274463</v>
+        <v>0.95954795385969993</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="E19" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
@@ -1071,26 +1087,26 @@
         <v>25</v>
       </c>
       <c r="C20" s="4">
-        <v>0.2</v>
+        <v>0.48</v>
       </c>
       <c r="D20">
         <f>C20*D$5</f>
-        <v>20</v>
+        <v>36.479999999999997</v>
       </c>
       <c r="E20">
         <f>D$4*2</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F20">
         <v>0.51</v>
       </c>
       <c r="H20" s="6">
         <f>F20*E20*D20</f>
-        <v>102</v>
+        <v>223.2576</v>
       </c>
       <c r="I20" s="8">
         <f t="shared" ref="I20:I23" si="3">H20/H$44</f>
-        <v>7.9751675176118278E-4</v>
+        <v>5.9505342395149978E-4</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
@@ -1098,26 +1114,26 @@
         <v>66</v>
       </c>
       <c r="C21" s="4">
-        <v>0.5</v>
+        <v>0.08</v>
       </c>
       <c r="D21">
         <f>C21*D$5</f>
-        <v>50</v>
+        <v>6.08</v>
       </c>
       <c r="E21">
         <f>D$4*2</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F21">
         <v>1.35</v>
       </c>
       <c r="H21" s="6">
         <f>F21*E21*D21</f>
-        <v>675</v>
+        <v>98.496000000000024</v>
       </c>
       <c r="I21" s="8">
         <f t="shared" si="3"/>
-        <v>5.2776843866548864E-3</v>
+        <v>2.6252356939036761E-4</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
@@ -1125,26 +1141,26 @@
         <v>26</v>
       </c>
       <c r="C22" s="4">
-        <v>0.3</v>
+        <v>0.45</v>
       </c>
       <c r="D22">
         <f>C22*D$5</f>
-        <v>30</v>
+        <v>34.200000000000003</v>
       </c>
       <c r="E22">
         <f>D$4*2</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F22">
         <v>6.29</v>
       </c>
       <c r="H22" s="6">
         <f>F22*E22*D22</f>
-        <v>1887</v>
+        <v>2581.4160000000002</v>
       </c>
       <c r="I22" s="8">
         <f t="shared" si="3"/>
-        <v>1.4754059907581883E-2</v>
+        <v>6.880305214439217E-3</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
@@ -1156,11 +1172,11 @@
       </c>
       <c r="D23">
         <f>C23*D$5</f>
-        <v>100</v>
+        <v>76</v>
       </c>
       <c r="E23">
         <f>D$4*2</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F23">
         <f>0.55/5</f>
@@ -1168,11 +1184,11 @@
       </c>
       <c r="H23" s="6">
         <f>F23*E23*D23</f>
-        <v>110.00000000000001</v>
+        <v>100.32000000000002</v>
       </c>
       <c r="I23" s="8">
         <f t="shared" si="3"/>
-        <v>8.6006708523264825E-4</v>
+        <v>2.6738511697167071E-4</v>
       </c>
       <c r="K23" s="5" t="s">
         <v>61</v>
@@ -1188,7 +1204,7 @@
       <c r="C24" s="4"/>
       <c r="J24" s="8">
         <f>SUM(I20:I23)</f>
-        <v>2.16893281312306E-2</v>
+        <v>8.0052673247527559E-3</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
@@ -1217,7 +1233,7 @@
       </c>
       <c r="D27">
         <f>C27*D$5</f>
-        <v>100</v>
+        <v>76</v>
       </c>
       <c r="E27">
         <v>1</v>
@@ -1227,11 +1243,11 @@
       </c>
       <c r="H27" s="6">
         <f>F27*D27*E27</f>
-        <v>600</v>
+        <v>456</v>
       </c>
       <c r="I27" s="8">
         <f t="shared" ref="I27:I40" si="4">H27/H$44</f>
-        <v>4.6912750103598987E-3</v>
+        <v>1.2153868953257757E-3</v>
       </c>
       <c r="J27" s="8"/>
       <c r="K27" t="s">
@@ -1247,7 +1263,7 @@
       </c>
       <c r="D28">
         <f>C28*D$5</f>
-        <v>100</v>
+        <v>76</v>
       </c>
       <c r="E28">
         <v>5</v>
@@ -1257,11 +1273,11 @@
       </c>
       <c r="H28" s="6">
         <f t="shared" ref="H28:H31" si="5">F28*D28*E28</f>
-        <v>450</v>
+        <v>342</v>
       </c>
       <c r="I28" s="8">
         <f t="shared" si="4"/>
-        <v>3.5184562577699244E-3</v>
+        <v>9.1154017149433172E-4</v>
       </c>
       <c r="J28" s="8"/>
       <c r="K28" t="s">
@@ -1280,7 +1296,7 @@
       </c>
       <c r="D29">
         <f>C29*D$5</f>
-        <v>200</v>
+        <v>152</v>
       </c>
       <c r="E29">
         <v>5</v>
@@ -1290,11 +1306,11 @@
       </c>
       <c r="H29" s="6">
         <f t="shared" si="5"/>
-        <v>7.0000000000000009</v>
+        <v>5.32</v>
       </c>
       <c r="I29" s="8">
         <f t="shared" si="4"/>
-        <v>5.4731541787532164E-5</v>
+        <v>1.4179513778800717E-5</v>
       </c>
       <c r="J29" s="8"/>
       <c r="K29" s="5" t="s">
@@ -1310,7 +1326,7 @@
       </c>
       <c r="D30">
         <f>C30*D$5</f>
-        <v>100</v>
+        <v>76</v>
       </c>
       <c r="E30" s="2">
         <v>100</v>
@@ -1320,11 +1336,11 @@
       </c>
       <c r="H30" s="6">
         <f t="shared" si="5"/>
-        <v>250</v>
+        <v>190</v>
       </c>
       <c r="I30" s="8">
         <f t="shared" si="4"/>
-        <v>1.9546979209832914E-3</v>
+        <v>5.0641120638573989E-4</v>
       </c>
       <c r="J30" s="8"/>
       <c r="K30" s="5" t="s">
@@ -1340,7 +1356,7 @@
       </c>
       <c r="D31" s="2">
         <f>C31*D$5</f>
-        <v>500</v>
+        <v>380</v>
       </c>
       <c r="E31" s="2">
         <v>5</v>
@@ -1350,11 +1366,11 @@
       </c>
       <c r="H31" s="6">
         <f t="shared" si="5"/>
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="I31" s="8">
         <f t="shared" si="4"/>
-        <v>1.9546979209832913E-4</v>
+        <v>5.0641120638573985E-5</v>
       </c>
       <c r="J31" s="8"/>
     </row>
@@ -1373,7 +1389,7 @@
       </c>
       <c r="J32" s="8">
         <f>SUM(I27:I31)</f>
-        <v>1.0414630522998977E-2</v>
+        <v>2.6981589076232218E-3</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.2">
@@ -1385,7 +1401,7 @@
       </c>
       <c r="D33">
         <f>C33*D$5</f>
-        <v>20</v>
+        <v>15.200000000000001</v>
       </c>
       <c r="E33">
         <v>8</v>
@@ -1395,11 +1411,11 @@
       </c>
       <c r="H33" s="6">
         <f>D33*E33*F33</f>
-        <v>16</v>
+        <v>12.160000000000002</v>
       </c>
       <c r="I33" s="8">
         <f t="shared" si="4"/>
-        <v>1.2510066694293063E-4</v>
+        <v>3.241031720868736E-5</v>
       </c>
       <c r="J33" s="8"/>
     </row>
@@ -1428,11 +1444,11 @@
       </c>
       <c r="D36">
         <f>C36*D$5</f>
-        <v>100</v>
+        <v>76</v>
       </c>
       <c r="E36">
         <f>D$4</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F36">
         <v>0.1125</v>
@@ -1442,11 +1458,11 @@
       </c>
       <c r="H36" s="6">
         <f>G36*F36*E36*D36</f>
-        <v>1125</v>
+        <v>1026</v>
       </c>
       <c r="I36" s="8">
         <f t="shared" si="4"/>
-        <v>8.7961406444248113E-3</v>
+        <v>2.7346205144829954E-3</v>
       </c>
       <c r="J36" s="8"/>
       <c r="K36" t="s">
@@ -1472,22 +1488,22 @@
       </c>
       <c r="D37">
         <f>C37*D$5</f>
-        <v>10</v>
+        <v>7.6000000000000005</v>
       </c>
       <c r="E37">
         <f>D$4</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F37">
         <v>7</v>
       </c>
       <c r="H37" s="6">
         <f>D37*F37*E37</f>
-        <v>350</v>
+        <v>319.20000000000005</v>
       </c>
       <c r="I37" s="8">
         <f t="shared" si="4"/>
-        <v>2.7365770893766077E-3</v>
+        <v>8.5077082672804305E-4</v>
       </c>
       <c r="J37" s="8"/>
       <c r="K37" t="s">
@@ -1503,22 +1519,22 @@
       </c>
       <c r="D38">
         <f>C38*D$5</f>
-        <v>40</v>
+        <v>30.400000000000002</v>
       </c>
       <c r="E38">
         <f>D$4</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F38">
         <v>12</v>
       </c>
       <c r="H38" s="6">
         <f>D38*F38*E38</f>
-        <v>2400</v>
+        <v>2188.8000000000002</v>
       </c>
       <c r="I38" s="8">
         <f t="shared" si="4"/>
-        <v>1.8765100041439595E-2</v>
+        <v>5.833857097563724E-3</v>
       </c>
       <c r="J38" s="8"/>
     </row>
@@ -1531,22 +1547,22 @@
       </c>
       <c r="D39">
         <f t="shared" ref="D39:D40" si="6">C39*D$5</f>
-        <v>30</v>
+        <v>22.8</v>
       </c>
       <c r="E39">
         <f t="shared" ref="E39:E40" si="7">D$4</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F39">
         <v>50</v>
       </c>
       <c r="H39" s="6">
         <f>D39*F39*E39</f>
-        <v>7500</v>
+        <v>6840</v>
       </c>
       <c r="I39" s="8">
         <f t="shared" si="4"/>
-        <v>5.8640937629498735E-2</v>
+        <v>1.8230803429886637E-2</v>
       </c>
       <c r="J39" s="8"/>
     </row>
@@ -1559,22 +1575,22 @@
       </c>
       <c r="D40">
         <f t="shared" si="6"/>
-        <v>20</v>
+        <v>15.200000000000001</v>
       </c>
       <c r="E40">
         <f t="shared" si="7"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F40">
         <v>8.5</v>
       </c>
       <c r="H40" s="6">
         <f>D40*F40*E40</f>
-        <v>850</v>
+        <v>775.2</v>
       </c>
       <c r="I40" s="8">
         <f t="shared" si="4"/>
-        <v>6.6459729313431901E-3</v>
+        <v>2.066157722053819E-3</v>
       </c>
       <c r="J40" s="8"/>
       <c r="K40" t="s">
@@ -1587,7 +1603,7 @@
       </c>
       <c r="J41" s="8">
         <f>SUM(I36:I40)</f>
-        <v>9.5584728336082947E-2</v>
+        <v>2.971620959071522E-2</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.2">
@@ -1596,7 +1612,7 @@
       </c>
       <c r="H44" s="6">
         <f>SUM(H8:H40)</f>
-        <v>127897</v>
+        <v>375189.16960000008</v>
       </c>
       <c r="I44" s="6" t="s">
         <v>47</v>
@@ -1608,7 +1624,7 @@
       </c>
       <c r="H45" s="6">
         <f>H44/D5</f>
-        <v>1278.97</v>
+        <v>4936.6996000000008</v>
       </c>
       <c r="I45" s="6" t="s">
         <v>47</v>
@@ -1704,7 +1720,7 @@
         <v>12</v>
       </c>
       <c r="I8" s="8">
-        <f>H8/H$42</f>
+        <f t="shared" ref="I8:I15" si="0">H8/H$42</f>
         <v>6.9613240438331364E-2</v>
       </c>
       <c r="J8" s="8"/>
@@ -1724,11 +1740,11 @@
         <v>4</v>
       </c>
       <c r="H9" s="6">
-        <f t="shared" ref="H9:H15" si="0">F9*E9*G9</f>
+        <f t="shared" ref="H9:H15" si="1">F9*E9*G9</f>
         <v>0</v>
       </c>
       <c r="I9" s="8">
-        <f>H9/H$42</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J9" s="8"/>
@@ -1747,11 +1763,11 @@
         <v>2</v>
       </c>
       <c r="H10" s="6">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="I10" s="8">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="I10" s="8">
-        <f>H10/H$42</f>
         <v>2.320441347944379E-2</v>
       </c>
       <c r="J10" s="8"/>
@@ -1773,11 +1789,11 @@
         <v>2</v>
       </c>
       <c r="H11" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I11" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I11" s="8">
-        <f>H11/H$42</f>
         <v>0</v>
       </c>
       <c r="J11" s="8"/>
@@ -1794,11 +1810,11 @@
         <v>2</v>
       </c>
       <c r="H12" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I12" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I12" s="8">
-        <f>H12/H$42</f>
         <v>0</v>
       </c>
       <c r="J12" s="8"/>
@@ -1818,11 +1834,11 @@
         <v>20</v>
       </c>
       <c r="H13" s="6">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="I13" s="8">
         <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-      <c r="I13" s="8">
-        <f>H13/H$42</f>
         <v>0.23204413479443789</v>
       </c>
       <c r="J13" s="8"/>
@@ -1840,11 +1856,11 @@
         <v>20</v>
       </c>
       <c r="H14" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I14" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I14" s="8">
-        <f>H14/H$42</f>
         <v>0</v>
       </c>
       <c r="J14" s="8"/>
@@ -1864,11 +1880,11 @@
         <v>3.3333333333333333E-2</v>
       </c>
       <c r="H15" s="6">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="I15" s="8">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="I15" s="8">
-        <f>H15/H$42</f>
         <v>1.1602206739721895E-2</v>
       </c>
       <c r="J15" s="8"/>
@@ -1904,7 +1920,7 @@
         <v>2.04</v>
       </c>
       <c r="I18" s="8">
-        <f t="shared" ref="I18:I21" si="1">H18/H$42</f>
+        <f t="shared" ref="I18:I21" si="2">H18/H$42</f>
         <v>1.1834250874516334E-2</v>
       </c>
     </row>
@@ -1919,11 +1935,11 @@
         <v>1.35</v>
       </c>
       <c r="H19" s="6">
-        <f t="shared" ref="H19:H21" si="2">F19*E19</f>
+        <f t="shared" ref="H19:H21" si="3">F19*E19</f>
         <v>4.0500000000000007</v>
       </c>
       <c r="I19" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.3494468647936841E-2</v>
       </c>
     </row>
@@ -1938,11 +1954,11 @@
         <v>6.29</v>
       </c>
       <c r="H20" s="6">
+        <f t="shared" si="3"/>
+        <v>18.87</v>
+      </c>
+      <c r="I20" s="8">
         <f t="shared" si="2"/>
-        <v>18.87</v>
-      </c>
-      <c r="I20" s="8">
-        <f t="shared" si="1"/>
         <v>0.10946682058927609</v>
       </c>
     </row>
@@ -1959,11 +1975,11 @@
         <v>0.11000000000000001</v>
       </c>
       <c r="H21" s="6">
+        <f t="shared" si="3"/>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="I21" s="8">
         <f t="shared" si="2"/>
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="I21" s="8">
-        <f t="shared" si="1"/>
         <v>6.3812137068470429E-3</v>
       </c>
       <c r="K21" s="5" t="s">
@@ -2011,7 +2027,7 @@
         <v>6</v>
       </c>
       <c r="I25" s="8">
-        <f t="shared" ref="I25:I38" si="3">H25/H$42</f>
+        <f t="shared" ref="I25:I38" si="4">H25/H$42</f>
         <v>3.4806620219165682E-2</v>
       </c>
       <c r="J25" s="8"/>
@@ -2030,11 +2046,11 @@
         <v>0.9</v>
       </c>
       <c r="H26" s="6">
-        <f t="shared" ref="H26:H29" si="4">F26*E26</f>
+        <f t="shared" ref="H26:H29" si="5">F26*E26</f>
         <v>4.5</v>
       </c>
       <c r="I26" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.6104965164374265E-2</v>
       </c>
       <c r="J26" s="8"/>
@@ -2056,11 +2072,11 @@
         <v>7.0000000000000001E-3</v>
       </c>
       <c r="H27" s="6">
+        <f t="shared" si="5"/>
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="I27" s="8">
         <f t="shared" si="4"/>
-        <v>2.1000000000000001E-2</v>
-      </c>
-      <c r="I27" s="8">
-        <f t="shared" si="3"/>
         <v>1.2182317076707991E-4</v>
       </c>
       <c r="J27" s="8"/>
@@ -2079,11 +2095,11 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="H28" s="6">
+        <f t="shared" si="5"/>
+        <v>2.5</v>
+      </c>
+      <c r="I28" s="8">
         <f t="shared" si="4"/>
-        <v>2.5</v>
-      </c>
-      <c r="I28" s="8">
-        <f t="shared" si="3"/>
         <v>1.4502758424652368E-2</v>
       </c>
       <c r="J28" s="8"/>
@@ -2102,11 +2118,11 @@
         <v>0.01</v>
       </c>
       <c r="H29" s="6">
+        <f t="shared" si="5"/>
+        <v>0.05</v>
+      </c>
+      <c r="I29" s="8">
         <f t="shared" si="4"/>
-        <v>0.05</v>
-      </c>
-      <c r="I29" s="8">
-        <f t="shared" si="3"/>
         <v>2.9005516849304737E-4</v>
       </c>
       <c r="J29" s="8"/>
@@ -2138,7 +2154,7 @@
         <v>4</v>
       </c>
       <c r="I31" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.320441347944379E-2</v>
       </c>
       <c r="J31" s="8"/>
@@ -2177,7 +2193,7 @@
         <v>11.25</v>
       </c>
       <c r="I34" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6.5262412910935666E-2</v>
       </c>
       <c r="J34" s="8"/>
@@ -2210,7 +2226,7 @@
         <v>0</v>
       </c>
       <c r="I35" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J35" s="8"/>
@@ -2234,7 +2250,7 @@
         <v>60</v>
       </c>
       <c r="I36" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.34806620219165685</v>
       </c>
       <c r="J36" s="8"/>
@@ -2254,7 +2270,7 @@
         <v>0</v>
       </c>
       <c r="I37" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J37" s="8"/>
@@ -2275,7 +2291,7 @@
         <v>0</v>
       </c>
       <c r="I38" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J38" s="8"/>

</xml_diff>

<commit_message>
Build 38. Finalisation de la traduction et des textes de la version Congrès. Version Congrès fonctionnelle Meilleure gestion de la mise en page du graphe Mise en rouge des paramètres généraux lorsqu'ils sont à zéro
</commit_message>
<xml_diff>
--- a/DonneesConferences/CO2 conférences.xlsx
+++ b/DonneesConferences/CO2 conférences.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkaspari/Documents/Perso/Divers/Programmation/BilanCO2/DonneesConferences/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40B24B3E-5DAC-C24E-B2DC-D8BDE4E19625}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47A97B87-94EF-7348-9751-1E0AE8C80231}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="500" windowWidth="19400" windowHeight="17920" xr2:uid="{3BEFCCA0-4A47-A44A-9737-BA198179BEF7}"/>
+    <workbookView xWindow="620" yWindow="500" windowWidth="28800" windowHeight="16240" activeTab="1" xr2:uid="{3BEFCCA0-4A47-A44A-9737-BA198179BEF7}"/>
   </bookViews>
   <sheets>
     <sheet name="Collectif" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="74">
   <si>
     <t>Informations générales</t>
   </si>
@@ -253,6 +253,12 @@
   </si>
   <si>
     <t>Nombre max</t>
+  </si>
+  <si>
+    <t>par jour</t>
+  </si>
+  <si>
+    <t>jours</t>
   </si>
 </sst>
 </file>
@@ -658,8 +664,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00E0F975-A56E-D441-BC3D-3D4EC260A329}">
   <dimension ref="A1:P45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -756,7 +762,7 @@
       </c>
       <c r="I8" s="8">
         <f>H8/H$44</f>
-        <v>9.723095162606206E-4</v>
+        <v>9.7165999770526285E-4</v>
       </c>
       <c r="J8" s="8"/>
       <c r="K8">
@@ -793,7 +799,7 @@
       </c>
       <c r="I9" s="8">
         <f t="shared" ref="I9:I17" si="2">H9/H$44</f>
-        <v>1.2153868953257758E-4</v>
+        <v>1.2145749971315786E-4</v>
       </c>
       <c r="J9" s="8"/>
       <c r="K9">
@@ -827,7 +833,7 @@
       </c>
       <c r="I10" s="8">
         <f t="shared" si="2"/>
-        <v>6.0769344766288788E-5</v>
+        <v>6.0728749856578928E-5</v>
       </c>
       <c r="J10" s="8"/>
       <c r="K10">
@@ -864,7 +870,7 @@
       </c>
       <c r="I11" s="8">
         <f t="shared" si="2"/>
-        <v>8.224117991704416E-3</v>
+        <v>8.2186241472570146E-3</v>
       </c>
       <c r="J11" s="8"/>
       <c r="K11">
@@ -898,7 +904,7 @@
       </c>
       <c r="I12" s="8">
         <f t="shared" si="2"/>
-        <v>2.8966721005264321E-2</v>
+        <v>2.8947370764969286E-2</v>
       </c>
       <c r="J12" s="8"/>
       <c r="K12">
@@ -935,7 +941,7 @@
       </c>
       <c r="I13" s="8">
         <f t="shared" si="2"/>
-        <v>1.6043107018300237E-2</v>
+        <v>1.6032389962136837E-2</v>
       </c>
       <c r="J13" s="8"/>
       <c r="K13">
@@ -969,7 +975,7 @@
       </c>
       <c r="I14" s="8">
         <f t="shared" si="2"/>
-        <v>0.89981168795443811</v>
+        <v>0.89921059912636425</v>
       </c>
       <c r="J14" s="8"/>
       <c r="K14">
@@ -1004,9 +1010,16 @@
       </c>
       <c r="I15" s="8">
         <f t="shared" si="2"/>
-        <v>4.8615475813031028E-3</v>
+        <v>4.8582999885263137E-3</v>
       </c>
       <c r="J15" s="8"/>
+      <c r="K15">
+        <f>E15*F15*2</f>
+        <v>4</v>
+      </c>
+      <c r="L15" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
@@ -1035,7 +1048,7 @@
       </c>
       <c r="I16" s="8">
         <f t="shared" si="2"/>
-        <v>4.861547581303103E-4</v>
+        <v>4.8582999885263142E-4</v>
       </c>
       <c r="J16" s="8"/>
     </row>
@@ -1071,7 +1084,7 @@
       </c>
       <c r="J18" s="8">
         <f>SUM(I8:I17)</f>
-        <v>0.95954795385969993</v>
+        <v>0.95890696023538124</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
@@ -1106,7 +1119,7 @@
       </c>
       <c r="I20" s="8">
         <f t="shared" ref="I20:I23" si="3">H20/H$44</f>
-        <v>5.9505342395149978E-4</v>
+        <v>5.9465591859562082E-4</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
@@ -1133,7 +1146,7 @@
       </c>
       <c r="I21" s="8">
         <f t="shared" si="3"/>
-        <v>2.6252356939036761E-4</v>
+        <v>2.62348199380421E-4</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
@@ -1160,7 +1173,7 @@
       </c>
       <c r="I22" s="8">
         <f t="shared" si="3"/>
-        <v>6.880305214439217E-3</v>
+        <v>6.8757090587618658E-3</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
@@ -1188,7 +1201,7 @@
       </c>
       <c r="I23" s="8">
         <f t="shared" si="3"/>
-        <v>2.6738511697167071E-4</v>
+        <v>2.6720649936894732E-4</v>
       </c>
       <c r="K23" s="5" t="s">
         <v>61</v>
@@ -1204,7 +1217,7 @@
       <c r="C24" s="4"/>
       <c r="J24" s="8">
         <f>SUM(I20:I23)</f>
-        <v>8.0052673247527559E-3</v>
+        <v>7.9999196761068557E-3</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
@@ -1236,18 +1249,18 @@
         <v>76</v>
       </c>
       <c r="E27">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F27">
         <v>6</v>
       </c>
       <c r="H27" s="6">
         <f>F27*D27*E27</f>
-        <v>456</v>
+        <v>912</v>
       </c>
       <c r="I27" s="8">
         <f t="shared" ref="I27:I40" si="4">H27/H$44</f>
-        <v>1.2153868953257757E-3</v>
+        <v>2.4291499942631569E-3</v>
       </c>
       <c r="J27" s="8"/>
       <c r="K27" t="s">
@@ -1266,18 +1279,18 @@
         <v>76</v>
       </c>
       <c r="E28">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F28">
         <v>0.9</v>
       </c>
       <c r="H28" s="6">
         <f t="shared" ref="H28:H31" si="5">F28*D28*E28</f>
-        <v>342</v>
+        <v>136.80000000000001</v>
       </c>
       <c r="I28" s="8">
         <f t="shared" si="4"/>
-        <v>9.1154017149433172E-4</v>
+        <v>3.6437249913947358E-4</v>
       </c>
       <c r="J28" s="8"/>
       <c r="K28" t="s">
@@ -1310,7 +1323,7 @@
       </c>
       <c r="I29" s="8">
         <f t="shared" si="4"/>
-        <v>1.4179513778800717E-5</v>
+        <v>1.417004163320175E-5</v>
       </c>
       <c r="J29" s="8"/>
       <c r="K29" s="5" t="s">
@@ -1340,7 +1353,7 @@
       </c>
       <c r="I30" s="8">
         <f t="shared" si="4"/>
-        <v>5.0641120638573989E-4</v>
+        <v>5.0607291547149103E-4</v>
       </c>
       <c r="J30" s="8"/>
       <c r="K30" s="5" t="s">
@@ -1370,7 +1383,7 @@
       </c>
       <c r="I31" s="8">
         <f t="shared" si="4"/>
-        <v>5.0641120638573985E-5</v>
+        <v>5.0607291547149106E-5</v>
       </c>
       <c r="J31" s="8"/>
     </row>
@@ -1389,7 +1402,7 @@
       </c>
       <c r="J32" s="8">
         <f>SUM(I27:I31)</f>
-        <v>2.6981589076232218E-3</v>
+        <v>3.3643727420544721E-3</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.2">
@@ -1415,7 +1428,7 @@
       </c>
       <c r="I33" s="8">
         <f t="shared" si="4"/>
-        <v>3.241031720868736E-5</v>
+        <v>3.2388666590175435E-5</v>
       </c>
       <c r="J33" s="8"/>
     </row>
@@ -1428,6 +1441,9 @@
       <c r="J34" s="8"/>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="E35" t="s">
+        <v>73</v>
+      </c>
       <c r="G35" t="s">
         <v>58</v>
       </c>
@@ -1462,7 +1478,7 @@
       </c>
       <c r="I36" s="8">
         <f t="shared" si="4"/>
-        <v>2.7346205144829954E-3</v>
+        <v>2.7327937435460514E-3</v>
       </c>
       <c r="J36" s="8"/>
       <c r="K36" t="s">
@@ -1503,7 +1519,7 @@
       </c>
       <c r="I37" s="8">
         <f t="shared" si="4"/>
-        <v>8.5077082672804305E-4</v>
+        <v>8.5020249799210512E-4</v>
       </c>
       <c r="J37" s="8"/>
       <c r="K37" t="s">
@@ -1534,7 +1550,7 @@
       </c>
       <c r="I38" s="8">
         <f t="shared" si="4"/>
-        <v>5.833857097563724E-3</v>
+        <v>5.8299599862315773E-3</v>
       </c>
       <c r="J38" s="8"/>
     </row>
@@ -1562,7 +1578,7 @@
       </c>
       <c r="I39" s="8">
         <f t="shared" si="4"/>
-        <v>1.8230803429886637E-2</v>
+        <v>1.8218624956973677E-2</v>
       </c>
       <c r="J39" s="8"/>
     </row>
@@ -1590,7 +1606,7 @@
       </c>
       <c r="I40" s="8">
         <f t="shared" si="4"/>
-        <v>2.066157722053819E-3</v>
+        <v>2.0647774951236837E-3</v>
       </c>
       <c r="J40" s="8"/>
       <c r="K40" t="s">
@@ -1603,7 +1619,7 @@
       </c>
       <c r="J41" s="8">
         <f>SUM(I36:I40)</f>
-        <v>2.971620959071522E-2</v>
+        <v>2.9696358679867092E-2</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.2">
@@ -1612,7 +1628,7 @@
       </c>
       <c r="H44" s="6">
         <f>SUM(H8:H40)</f>
-        <v>375189.16960000008</v>
+        <v>375439.96960000007</v>
       </c>
       <c r="I44" s="6" t="s">
         <v>47</v>
@@ -1624,7 +1640,7 @@
       </c>
       <c r="H45" s="6">
         <f>H44/D5</f>
-        <v>4936.6996000000008</v>
+        <v>4939.999600000001</v>
       </c>
       <c r="I45" s="6" t="s">
         <v>47</v>
@@ -1644,8 +1660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4A32ACA-C7FB-9D48-A4D3-4B05A7AEEF25}">
   <dimension ref="A1:P43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="W49" sqref="W49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>